<commit_message>
add show missing drawings + comma for prices
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -470,6 +470,11 @@
           <t>Material</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Kosten in €</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -498,7 +503,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Kosten in €</t>
+          <t>10,96</t>
         </is>
       </c>
     </row>
@@ -529,7 +534,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>5.48</t>
+          <t>5,48</t>
         </is>
       </c>
     </row>
@@ -560,7 +565,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>43.84</t>
+          <t>43,84</t>
         </is>
       </c>
     </row>
@@ -591,7 +596,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>67.20</t>
+          <t>67,20</t>
         </is>
       </c>
     </row>
@@ -622,7 +627,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>16.80</t>
+          <t>16,80</t>
         </is>
       </c>
     </row>
@@ -653,7 +658,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>67.20</t>
+          <t>67,20</t>
         </is>
       </c>
     </row>
@@ -684,7 +689,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>33.60</t>
+          <t>33,60</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix bug convert speed to mm/s
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -424,16 +424,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col width="12.28515625" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="18.7109375" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="33.42578125" customWidth="1" min="3" max="3"/>
     <col width="25" bestFit="1" customWidth="1" min="4" max="4"/>
     <col width="5.85546875" customWidth="1" min="5" max="5"/>
     <col width="8.42578125" bestFit="1" customWidth="1" min="6" max="6"/>
@@ -485,7 +485,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>L00009630</t>
+          <t>MM00235120_Knotenblech.dxf</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -503,7 +503,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>10,96</t>
+          <t>2,82</t>
         </is>
       </c>
     </row>
@@ -516,7 +516,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>L00009642</t>
+          <t>L00040312_Halterung.dxf</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -534,162 +534,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>5,48</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="n">
-        <v>4</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>L00009648</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Verstärkungsblech</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>10</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>S235JR</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>43,84</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="n">
-        <v>4</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>L00009661</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Begrenzung vorn</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>15</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>S235JR</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>67,20</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>L00011235</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Halterung Getriebe</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>15</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>S235JR</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>16,80</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="n">
-        <v>4</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>L00009727</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Zylinderauge</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>15</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>S355J2</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>67,20</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>L00033773</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Füllstückhalterung</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>15</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>S235JR</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>33,60</t>
+          <t>0,79</t>
         </is>
       </c>
     </row>

</xml_diff>